<commit_message>
COST AFFIDAVIT CHANGES AND EXCEL CHANGES
</commit_message>
<xml_diff>
--- a/bin/com/ptl/data/TestData Excel.xlsx
+++ b/bin/com/ptl/data/TestData Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="13365" windowHeight="4755" tabRatio="700" firstSheet="17" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11310" windowHeight="4050" tabRatio="700" firstSheet="18" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="6" r:id="rId1"/>
@@ -33,12 +33,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K14"/>
+  <oleSize ref="A1:I12"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="230">
   <si>
     <t>Task 1</t>
   </si>
@@ -718,34 +718,16 @@
     <t>0112999922</t>
   </si>
   <si>
-    <t>StatementNo</t>
-  </si>
-  <si>
     <t>FTS</t>
   </si>
   <si>
-    <t>To Date</t>
-  </si>
-  <si>
-    <t>D/COM/R/00012</t>
-  </si>
-  <si>
-    <t>Less than 2 weeks old, for breeding</t>
-  </si>
-  <si>
-    <t>Kilogram</t>
-  </si>
-  <si>
-    <t>25/8/2015</t>
-  </si>
-  <si>
     <t>CostState New</t>
   </si>
   <si>
     <t>Creates new Cost Statement</t>
   </si>
   <si>
-    <t>27/8/2015</t>
+    <t xml:space="preserve">Cost Statement </t>
   </si>
 </sst>
 </file>
@@ -855,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -874,7 +856,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1406,13 +1387,13 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>233</v>
+      <c r="A18" s="18" t="s">
+        <v>227</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="C18" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -2278,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2823,8 +2804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,19 +2827,19 @@
         <v>9</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>226</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>94</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>188</v>
@@ -2873,51 +2854,57 @@
         <v>183</v>
       </c>
       <c r="L1" s="8" t="s">
-        <v>228</v>
+        <v>98</v>
       </c>
       <c r="M1" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
         <v>87</v>
       </c>
-      <c r="D2" t="s">
-        <v>74</v>
+      <c r="E2" t="s">
+        <v>229</v>
       </c>
       <c r="F2" t="s">
-        <v>229</v>
+        <v>182</v>
       </c>
       <c r="G2" t="s">
         <v>93</v>
       </c>
       <c r="H2" t="s">
-        <v>230</v>
-      </c>
-      <c r="I2">
-        <v>500</v>
+        <v>184</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="J2" t="s">
-        <v>231</v>
-      </c>
-      <c r="K2" t="s">
-        <v>232</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>235</v>
+        <v>82</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="M2" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="suranga1@yahoo.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
code changes to: TestPages(ApplyCOOPage) Testcases(SaveNewCOOTest and ResubmitRevertedApplicationTest)
</commit_message>
<xml_diff>
--- a/bin/com/ptl/data/TestData Excel.xlsx
+++ b/bin/com/ptl/data/TestData Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="11310" windowHeight="4050" tabRatio="700" firstSheet="18" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="8520" windowHeight="4845" tabRatio="700" firstSheet="9" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="6" r:id="rId1"/>
@@ -33,7 +33,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:I12"/>
+  <oleSize ref="A1:J14"/>
 </workbook>
 </file>
 
@@ -837,7 +837,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -857,6 +857,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1566,7 +1567,7 @@
   <dimension ref="A1:AF2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,14 +1776,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" customFormat="1" x14ac:dyDescent="0.25">
@@ -1890,8 +1894,8 @@
       <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" t="s">
-        <v>136</v>
+      <c r="D2" s="19" t="s">
+        <v>93</v>
       </c>
       <c r="E2" t="s">
         <v>137</v>
@@ -1977,6 +1981,7 @@
     <hyperlink ref="B2" r:id="rId1" display="suranga1@yahoo.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2804,7 +2809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updates to classes : Pages(HomePage, CitizeHomePage) TestCases(LoginTest, LogoutTest, CitizenLogoutTest)
</commit_message>
<xml_diff>
--- a/bin/com/ptl/data/TestData Excel.xlsx
+++ b/bin/com/ptl/data/TestData Excel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="8520" windowHeight="4845" tabRatio="700" firstSheet="9" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="11760" windowHeight="4020" tabRatio="700"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="6" r:id="rId1"/>
@@ -33,12 +33,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J14"/>
+  <oleSize ref="A7:G18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="234">
   <si>
     <t>Task 1</t>
   </si>
@@ -728,6 +728,18 @@
   </si>
   <si>
     <t xml:space="preserve">Cost Statement </t>
+  </si>
+  <si>
+    <t>Logout Test</t>
+  </si>
+  <si>
+    <t>User log out test</t>
+  </si>
+  <si>
+    <t>Logout Test Citizen</t>
+  </si>
+  <si>
+    <t>Logout Test for citizen application</t>
   </si>
 </sst>
 </file>
@@ -1191,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,10 +1251,10 @@
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>11</v>
+        <v>230</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>16</v>
+        <v>231</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>19</v>
@@ -1250,10 +1262,10 @@
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>12</v>
+        <v>232</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>17</v>
+        <v>233</v>
       </c>
       <c r="C5" s="15" t="s">
         <v>19</v>
@@ -1261,10 +1273,10 @@
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>19</v>
@@ -1272,10 +1284,10 @@
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>61</v>
+        <v>17</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>19</v>
@@ -1283,74 +1295,74 @@
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B11" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C9" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="C11" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B12" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>177</v>
+        <v>99</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>179</v>
+        <v>113</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>19</v>
@@ -1358,10 +1370,10 @@
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>19</v>
@@ -1369,32 +1381,54 @@
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B18" s="14" t="s">
         <v>196</v>
       </c>
-      <c r="C16" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="C18" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="B17"/>
-      <c r="C17" s="10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="B19"/>
+      <c r="C19" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>227</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B20" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C20" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1776,7 +1810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -2698,7 +2732,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>